<commit_message>
Bring up to date 8-20-18
everything all at once
</commit_message>
<xml_diff>
--- a/CLRS_Session/Images/xydata.xlsx
+++ b/CLRS_Session/Images/xydata.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\GitHub\IBNR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\GitHub\IBNR\CLRS_Session\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A110BF-03C3-4495-94E6-75387564975F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A7C7E7-701F-4707-B41E-AC75FEC43B6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20710" windowHeight="3810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t/>
   </si>
@@ -81,16 +82,69 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aggregated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -112,8 +166,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -153,7 +221,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment wrapText="1"/>
@@ -276,6 +344,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -598,9 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -815,6 +890,304 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C352BC36-03F2-4112-8644-0BF9DC019E85}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.81640625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="40"/>
+      <c r="B1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="41">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35">
+        <v>129.2764</v>
+      </c>
+      <c r="C2" s="38">
+        <v>218.24</v>
+      </c>
+      <c r="E2" s="43">
+        <f>SUM(B2:B5)</f>
+        <v>436.6096</v>
+      </c>
+      <c r="F2" s="43">
+        <f>SUM(C2:C5)</f>
+        <v>871.56999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="41">
+        <v>2</v>
+      </c>
+      <c r="B3" s="35">
+        <v>135.47329999999999</v>
+      </c>
+      <c r="C3" s="38">
+        <v>255.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="41">
+        <v>3</v>
+      </c>
+      <c r="B4" s="35">
+        <v>94.534800000000004</v>
+      </c>
+      <c r="C4" s="38">
+        <v>232.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="41">
+        <v>4</v>
+      </c>
+      <c r="B5" s="35">
+        <v>77.325100000000006</v>
+      </c>
+      <c r="C5" s="38">
+        <v>165.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="41">
+        <v>5</v>
+      </c>
+      <c r="B6" s="35">
+        <v>130.2944</v>
+      </c>
+      <c r="C6" s="38">
+        <v>296.19</v>
+      </c>
+      <c r="E6" s="43">
+        <f>SUM(B6:B9)</f>
+        <v>357.09230000000002</v>
+      </c>
+      <c r="F6" s="43">
+        <f>SUM(C6:C9)</f>
+        <v>680.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="41">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35">
+        <v>9.1021999999999998</v>
+      </c>
+      <c r="C7" s="38">
+        <v>35.770000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="41">
+        <v>7</v>
+      </c>
+      <c r="B8" s="35">
+        <v>131.50489999999999</v>
+      </c>
+      <c r="C8" s="38">
+        <v>233.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="41">
+        <v>8</v>
+      </c>
+      <c r="B9" s="35">
+        <v>86.190799999999996</v>
+      </c>
+      <c r="C9" s="38">
+        <v>114.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="41">
+        <v>9</v>
+      </c>
+      <c r="B10" s="35">
+        <v>85.792000000000002</v>
+      </c>
+      <c r="C10" s="38">
+        <v>112.39</v>
+      </c>
+      <c r="E10" s="43">
+        <f>SUM(B10:B13)</f>
+        <v>424.87909999999999</v>
+      </c>
+      <c r="F10" s="43">
+        <f>SUM(C10:C13)</f>
+        <v>859.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="41">
+        <v>10</v>
+      </c>
+      <c r="B11" s="35">
+        <v>54.033900000000003</v>
+      </c>
+      <c r="C11" s="38">
+        <v>161.13999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="41">
+        <v>11</v>
+      </c>
+      <c r="B12" s="35">
+        <v>94.187600000000003</v>
+      </c>
+      <c r="C12" s="38">
+        <v>169.68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="41">
+        <v>12</v>
+      </c>
+      <c r="B13" s="35">
+        <v>190.8656</v>
+      </c>
+      <c r="C13" s="38">
+        <v>416.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="41">
+        <v>13</v>
+      </c>
+      <c r="B14" s="35">
+        <v>118.5314</v>
+      </c>
+      <c r="C14" s="38">
+        <v>263.72000000000003</v>
+      </c>
+      <c r="E14" s="43">
+        <f>SUM(B14:B17)</f>
+        <v>447.86059999999998</v>
+      </c>
+      <c r="F14" s="43">
+        <f>SUM(C14:C17)</f>
+        <v>1045.0500000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="41">
+        <v>14</v>
+      </c>
+      <c r="B15" s="35">
+        <v>126.0108</v>
+      </c>
+      <c r="C15" s="38">
+        <v>244.73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="41">
+        <v>15</v>
+      </c>
+      <c r="B16" s="35">
+        <v>62.473399999999998</v>
+      </c>
+      <c r="C16" s="38">
+        <v>150.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="41">
+        <v>16</v>
+      </c>
+      <c r="B17" s="35">
+        <v>140.845</v>
+      </c>
+      <c r="C17" s="38">
+        <v>385.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="44">
+        <v>17</v>
+      </c>
+      <c r="B18" s="45">
+        <v>77.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="44">
+        <v>18</v>
+      </c>
+      <c r="B19" s="45">
+        <v>131.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="43">
+        <f>SUM(B2:B17)</f>
+        <v>1666.4416000000003</v>
+      </c>
+      <c r="C21" s="43">
+        <f>SUM(C2:C17)</f>
+        <v>3455.95</v>
+      </c>
+      <c r="E21" s="43">
+        <f>SUM(E2:E17)</f>
+        <v>1666.4416000000001</v>
+      </c>
+      <c r="F21" s="43">
+        <f>SUM(F2:F17)</f>
+        <v>3455.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="7" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="46">
+        <f>C21/B21</f>
+        <v>2.0738500527111174</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="46">
+        <f>F21/E21</f>
+        <v>2.0738500527111179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E14:F14 E2:F10" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>

</xml_diff>